<commit_message>
A bit more structural work in preperation for all of the R5900 instruction implementations.
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/R5900 Instruction Implementation Register.xlsx
+++ b/PCSX2_Core/Docs/R5900 Instruction Implementation Register.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\Dev\Projects\PCSX2_Rewrite\PCSX2_Core\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\Dev\Projects\PCSX2_Rewrite\PCSX2_Core\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" tabRatio="786" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" tabRatio="786" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="3" r:id="rId1"/>
@@ -1644,7 +1644,7 @@
         <v>314</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H34" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
+        <f t="shared" ref="H2" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
         <v>{Class Index, Type, Mnemonic, Implementation Index, Branch Delay Type, Cycles, Lookup Function (Pointer to)},</v>
       </c>
     </row>
@@ -2602,7 +2602,7 @@
         <v>314</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H34" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
+        <f t="shared" ref="H2" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
         <v>{Class Index, Type, Mnemonic, Implementation Index, Branch Delay Type, Cycles, Lookup Function (Pointer to)},</v>
       </c>
     </row>
@@ -5366,7 +5366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -5414,7 +5414,7 @@
         <v>314</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H34" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
+        <f t="shared" ref="H2" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
         <v>{Class Index, Type, Mnemonic, Implementation Index, Branch Delay Type, Cycles, Lookup Function (Pointer to)},</v>
       </c>
     </row>
@@ -6372,7 +6372,7 @@
         <v>314</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H34" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
+        <f t="shared" ref="H2" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
         <v>{Class Index, Type, Mnemonic, Implementation Index, Branch Delay Type, Cycles, Lookup Function (Pointer to)},</v>
       </c>
     </row>
@@ -7329,7 +7329,7 @@
         <v>314</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H65" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
+        <f t="shared" ref="H2" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
         <v>{Class Index, Type, Mnemonic, Implementation Index, Branch Delay Type, Cycles, Lookup Function (Pointer to)},</v>
       </c>
     </row>
@@ -9182,7 +9182,7 @@
         <v>314</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H65" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
+        <f t="shared" ref="H2" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
         <v>{Class Index, Type, Mnemonic, Implementation Index, Branch Delay Type, Cycles, Lookup Function (Pointer to)},</v>
       </c>
     </row>
@@ -10987,9 +10987,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3:H3"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18510,7 +18510,7 @@
         <v>314</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H34" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
+        <f t="shared" ref="H2" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
         <v>{Class Index, Type, Mnemonic, Implementation Index, Branch Delay Type, Cycles, Lookup Function (Pointer to)},</v>
       </c>
     </row>
@@ -19468,7 +19468,7 @@
         <v>314</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H34" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
+        <f t="shared" ref="H2" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
         <v>{Class Index, Type, Mnemonic, Implementation Index, Branch Delay Type, Cycles, Lookup Function (Pointer to)},</v>
       </c>
     </row>
@@ -20426,7 +20426,7 @@
         <v>314</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H34" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
+        <f t="shared" ref="H2" si="0">"{"&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;IF(ISBLANK(G2),"nullptr",G2)&amp;"},"</f>
         <v>{Class Index, Type, Mnemonic, Implementation Index, Branch Delay Type, Cycles, Lookup Function (Pointer to)},</v>
       </c>
     </row>

</xml_diff>